<commit_message>
Servidor Montado en NodeJS-Conexion BD
Servicios para persona (CRUD), conxion local a BD
</commit_message>
<xml_diff>
--- a/Documentacion/ev1_plantillastakeholders.xlsx
+++ b/Documentacion/ev1_plantillastakeholders.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIO\Documents\Proyectos\E-vote\E-vote-Backend\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\E-vote\E-vote-Backend\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0E01C8-4E06-476B-9C47-6B65FA52A980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plantillaStakeHolders" sheetId="2" r:id="rId1"/>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Amparo</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="181">
   <si>
     <t>NOMBRE DE LA ORGANIZACIÓN</t>
   </si>
@@ -701,11 +702,26 @@
   <si>
     <t>Generar reporte de votación</t>
   </si>
+  <si>
+    <t>5.5.51</t>
+  </si>
+  <si>
+    <t>10.16.0</t>
+  </si>
+  <si>
+    <t>1.40.1</t>
+  </si>
+  <si>
+    <t>SAT LD101</t>
+  </si>
+  <si>
+    <t>U Are 4500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1156,11 +1172,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1188,27 +1225,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,7 +1255,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1253,6 +1269,204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>367394</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>54427</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>622007</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>370607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06F0BF6C-C9E3-4E7F-A7CF-A01484389454}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13838465" y="8313963"/>
+          <a:ext cx="5792721" cy="4724894"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3464626</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>176297</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F592832F-E6C2-4E3D-AABB-3006B26AD7B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10368644" y="8504465"/>
+          <a:ext cx="3056411" cy="3959082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>843644</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>8165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>874524</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A41C51-1F5E-40B0-B8FB-869B2FB82D9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14292944" y="14067065"/>
+          <a:ext cx="4602880" cy="2277835"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>734784</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>272143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247269</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Lector de Huella U are U 4500 es el dispositivo de sensor de hueva óptico mediante usb">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{239DBECD-B612-4703-844D-2A1011913C59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10695213" y="13770429"/>
+          <a:ext cx="3023127" cy="2598964"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1331,6 +1545,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1366,6 +1597,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1541,16 +1789,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="56.7109375" style="1" hidden="1" customWidth="1"/>
@@ -1565,51 +1813,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
     </row>
     <row r="4" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1774,14 +2022,14 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1790,261 +2038,282 @@
       <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
     </row>
     <row r="13" spans="1:11" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="14" spans="1:11" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:11" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-    </row>
-    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-    </row>
-    <row r="20" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+    </row>
+    <row r="20" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-    </row>
-    <row r="22" spans="1:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+    </row>
+    <row r="22" spans="1:7" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-    </row>
-    <row r="23" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+    </row>
+    <row r="23" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-    </row>
-    <row r="24" spans="1:6" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+    </row>
+    <row r="24" spans="1:7" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-    </row>
-    <row r="25" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+    </row>
+    <row r="25" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>179</v>
+      </c>
       <c r="B29" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>180</v>
+      </c>
       <c r="B30" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>176</v>
+      </c>
       <c r="B32" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="23" t="s">
+        <v>177</v>
+      </c>
       <c r="B33" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="56"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="23" t="s">
+        <v>178</v>
+      </c>
       <c r="B34" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="56"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="45"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C34:F34"/>
     <mergeCell ref="C14:F14"/>
@@ -2061,29 +2330,20 @@
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C3:C25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,6 +2585,11 @@
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="21"/>
     </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1117544613</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2333,7 +2598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>